<commit_message>
Get Reports to RUn
</commit_message>
<xml_diff>
--- a/src/test/resources/obieeReportsExcel/Test Data Reports.xlsx
+++ b/src/test/resources/obieeReportsExcel/Test Data Reports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\SeleniumTraining\ReportTestingOBIEE\src\test\resources\obieeReportsExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ReportTestingMulti\src\test\resources\obieeReportsExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B0C8AA-1C0D-470D-9A3E-C4CE19ED6758}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3879372D-756D-4314-802E-4B3BC66A9EF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20052" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="15" activeTab="17" xr2:uid="{63C22002-1F04-49DB-8E42-A4464D5F3BA0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="21" activeTab="24" xr2:uid="{63C22002-1F04-49DB-8E42-A4464D5F3BA0}"/>
   </bookViews>
   <sheets>
     <sheet name="StatusSummary" sheetId="1" r:id="rId1"/>
@@ -810,20 +810,20 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <col min="8" max="8" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -900,14 +900,14 @@
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <col min="4" max="4" width="19.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -921,7 +921,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -948,14 +948,14 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="3" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -972,7 +972,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -1002,14 +1002,14 @@
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1050,14 +1050,14 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1098,14 +1098,14 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1146,15 +1146,15 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="24.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1195,17 +1195,17 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1223,17 +1223,17 @@
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1247,17 +1247,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A5E0D0-4C1D-449A-9779-95652DE25E94}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="18.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -1298,14 +1298,14 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1340,13 +1340,13 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="3" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1387,15 +1387,15 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="18.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1442,14 +1442,14 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1484,14 +1484,14 @@
       <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1532,16 +1532,16 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="24.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>122</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1588,14 +1588,14 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>107</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1626,19 +1626,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA6124C-C6AC-4817-BDB0-3208AEA7C24B}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="27.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <col min="4" max="4" width="19.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>42736</v>
       </c>
       <c r="D2" s="1">
-        <v>43799</v>
+        <v>43830</v>
       </c>
     </row>
   </sheetData>
@@ -1679,14 +1679,14 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="26.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>110</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -1721,14 +1721,14 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="26.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -1763,20 +1763,20 @@
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1859,15 +1859,15 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.86328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <col min="4" max="4" width="14.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1908,15 +1908,15 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1957,14 +1957,14 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>24</v>
       </c>
@@ -2005,15 +2005,15 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -2054,16 +2054,16 @@
       <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <col min="6" max="7" width="20.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -2122,20 +2122,20 @@
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>

</xml_diff>